<commit_message>
*download done *delete all activities *hide assess button
</commit_message>
<xml_diff>
--- a/public/hello world.xlsx
+++ b/public/hello world.xlsx
@@ -7,7 +7,7 @@
     <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
+    <sheet name="CKP-R" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
   <si>
     <t>CKP-R</t>
   </si>
@@ -120,6 +120,18 @@
   </si>
   <si>
     <t>Mengikuti pelatihan sakernas add</t>
+  </si>
+  <si>
+    <t>Pegawai yang Dinilai</t>
+  </si>
+  <si>
+    <t>Pejabat Penilai</t>
+  </si>
+  <si>
+    <t>Indra</t>
+  </si>
+  <si>
+    <t>Iva</t>
   </si>
 </sst>
 </file>
@@ -268,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -277,6 +289,9 @@
     </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
@@ -622,17 +637,17 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A16" sqref="A16:J16"/>
+      <selection activeCell="B19" sqref="B19:I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="true" style="0"/>
     <col min="2" max="2" width="22" customWidth="true" style="0"/>
-    <col min="3" max="3" width="80" customWidth="true" style="0"/>
+    <col min="3" max="3" width="65" customWidth="true" style="0"/>
     <col min="4" max="4" width="15" customWidth="true" style="0"/>
     <col min="5" max="5" width="15" customWidth="true" style="0"/>
     <col min="6" max="6" width="15" customWidth="true" style="0"/>
@@ -685,184 +700,262 @@
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5" t="s">
+      <c r="C9" s="6"/>
+      <c r="D9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5" t="s">
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="J9" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="4"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6" t="s">
+      <c r="A10" s="5"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="8"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="9"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10" t="s">
+      <c r="C11" s="11"/>
+      <c r="D11" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="I11" s="10" t="s">
+      <c r="I11" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="J11" s="11" t="s">
+      <c r="J11" s="12" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13" t="s">
+      <c r="A12" s="13"/>
+      <c r="B12" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="15"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="15">
+      <c r="A13" s="16">
         <v>1</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16" t="s">
+      <c r="C13" s="17"/>
+      <c r="D13" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="16">
+      <c r="E13" s="17">
         <v>1.0</v>
       </c>
-      <c r="F13" s="16">
+      <c r="F13" s="17">
         <v>1.0</v>
       </c>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16">
+      <c r="G13" s="17"/>
+      <c r="H13" s="17">
         <v>100.0</v>
       </c>
-      <c r="I13" s="16"/>
-      <c r="J13" s="17" t="s">
+      <c r="I13" s="17"/>
+      <c r="J13" s="18" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="15">
+      <c r="A14" s="16">
         <v>2</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16" t="s">
+      <c r="C14" s="17"/>
+      <c r="D14" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="16">
+      <c r="E14" s="17">
         <v>1.0</v>
       </c>
-      <c r="F14" s="16">
+      <c r="F14" s="17">
         <v>1.0</v>
       </c>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16">
+      <c r="G14" s="17"/>
+      <c r="H14" s="17">
         <v>100.0</v>
       </c>
-      <c r="I14" s="16"/>
-      <c r="J14" s="17" t="s">
+      <c r="I14" s="17"/>
+      <c r="J14" s="18" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="12"/>
-      <c r="B15" s="13" t="s">
+      <c r="A15" s="13"/>
+      <c r="B15" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="15"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="15">
+      <c r="A16" s="16">
         <v>1</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16" t="s">
+      <c r="C16" s="17"/>
+      <c r="D16" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="16">
+      <c r="E16" s="17">
         <v>1.0</v>
       </c>
-      <c r="F16" s="16">
+      <c r="F16" s="17">
         <v>1.0</v>
       </c>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16">
+      <c r="G16" s="17"/>
+      <c r="H16" s="17">
         <v>100.0</v>
       </c>
-      <c r="I16" s="16"/>
-      <c r="J16" s="17" t="s">
+      <c r="I16" s="17"/>
+      <c r="J16" s="18" t="s">
         <v>31</v>
       </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="B19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I19" s="3"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="B24" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
@@ -881,6 +974,20 @@
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:J15"/>
     <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="H25:I25"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>